<commit_message>
gw update the form
</commit_message>
<xml_diff>
--- a/LF/TAS/Guinee Bissau/2023/gw_lf_tas1_202310_3_fts_result.xlsx
+++ b/LF/TAS/Guinee Bissau/2023/gw_lf_tas1_202310_3_fts_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Guinee Bissau\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBD6890-C1C8-46CA-9ABC-07D72EC45402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD38544-D7D0-4617-8B5F-A55F9144E05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="130">
   <si>
     <t>type</t>
   </si>
@@ -351,30 +351,12 @@
     <t>d_code_id</t>
   </si>
   <si>
-    <t>d_code_id2</t>
-  </si>
-  <si>
     <t>Selecione o código do participante</t>
   </si>
   <si>
-    <t>Insira manualmente o código do participante</t>
-  </si>
-  <si>
-    <t>. = ${d_code_id}</t>
-  </si>
-  <si>
-    <t>O código repetido deve ser o mesmo</t>
-  </si>
-  <si>
     <t>d_eu</t>
   </si>
   <si>
-    <t>(Jan 2024) 3. TAS1 FL - Resultado FTS V1</t>
-  </si>
-  <si>
-    <t>gw_lf_tas1_202402_3_fts_result_v1</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -387,9 +369,6 @@
     <t>Resultado FTS</t>
   </si>
   <si>
-    <t>gw_fts_202402_v1</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -436,6 +415,15 @@
   </si>
   <si>
     <t>Este ID já foi introduzido!</t>
+  </si>
+  <si>
+    <t>(Jan 2024) 3. TAS1 FL - Resultado FTS V1.2</t>
+  </si>
+  <si>
+    <t>gw_lf_tas1_202402_3_fts_result_v1_2</t>
+  </si>
+  <si>
+    <t>gw_fts_202402_v1_2</t>
   </si>
 </sst>
 </file>
@@ -934,13 +922,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1039,7 +1027,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>100</v>
@@ -1129,7 +1117,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
@@ -1138,7 +1126,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="16"/>
       <c r="I7" s="15" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -1147,13 +1135,13 @@
     </row>
     <row r="8" spans="1:14" s="12" customFormat="1">
       <c r="A8" s="20" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="20"/>
@@ -1172,7 +1160,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
@@ -1181,7 +1169,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="16"/>
       <c r="I9" s="15" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
@@ -1193,7 +1181,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
@@ -1202,7 +1190,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="16"/>
       <c r="I10" s="15" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
@@ -1211,13 +1199,13 @@
     </row>
     <row r="11" spans="1:14" s="12" customFormat="1">
       <c r="A11" s="15" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="15"/>
@@ -1240,18 +1228,18 @@
         <v>104</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="15" t="s">
@@ -1261,51 +1249,49 @@
       <c r="L12" s="16"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="1:14" s="12" customFormat="1" ht="31.5">
+    <row r="13" spans="1:14" s="12" customFormat="1">
       <c r="A13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>105</v>
+      <c r="B13" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>109</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="16" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
       <c r="M13" s="15"/>
     </row>
     <row r="14" spans="1:14" s="12" customFormat="1">
       <c r="A14" s="15" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="26"/>
+        <v>31</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>32</v>
+      </c>
       <c r="E14" s="15"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="18"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="26"/>
       <c r="H14" s="16" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="I14" s="16"/>
       <c r="J14" s="15" t="s">
@@ -1317,22 +1303,20 @@
     </row>
     <row r="15" spans="1:14" s="12" customFormat="1">
       <c r="A15" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>32</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D15" s="26"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="26"/>
       <c r="H15" s="16" t="s">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="15" t="s">
@@ -1342,22 +1326,22 @@
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:14" s="12" customFormat="1">
+    <row r="16" spans="1:14" s="12" customFormat="1" ht="31.5">
       <c r="A16" s="15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="26"/>
       <c r="H16" s="16" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="I16" s="16"/>
       <c r="J16" s="15" t="s">
@@ -1367,24 +1351,22 @@
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:13" s="12" customFormat="1" ht="31.5">
+    <row r="17" spans="1:13" s="12" customFormat="1">
       <c r="A17" s="15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>39</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C17" s="18"/>
       <c r="D17" s="26"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="26"/>
-      <c r="H17" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="I17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="J17" s="15" t="s">
         <v>20</v>
       </c>
@@ -1392,99 +1374,101 @@
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="1:13" s="12" customFormat="1">
+    <row r="18" spans="1:13" s="12" customFormat="1" ht="63">
       <c r="A18" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="18"/>
+        <v>43</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="D18" s="26"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="26"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="H18" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="1:13" s="12" customFormat="1" ht="63">
+    <row r="19" spans="1:13" s="12" customFormat="1">
       <c r="A19" s="15" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="26"/>
+        <v>46</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="28"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>28</v>
+      </c>
       <c r="H19" s="16" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
+      <c r="J19" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="1:13" s="12" customFormat="1">
+    <row r="20" spans="1:13">
       <c r="A20" s="15" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>28</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="I20" s="15"/>
+        <v>121</v>
+      </c>
+      <c r="I20" s="27"/>
       <c r="J20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>50</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D21" s="28"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
       <c r="G21" s="28"/>
       <c r="H21" s="16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I21" s="27"/>
       <c r="J21" s="15" t="s">
@@ -1494,22 +1478,22 @@
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" ht="31.5">
       <c r="A22" s="15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
       <c r="G22" s="28"/>
       <c r="H22" s="16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I22" s="27"/>
       <c r="J22" s="15" t="s">
@@ -1519,117 +1503,113 @@
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
     </row>
-    <row r="23" spans="1:13" ht="31.5">
+    <row r="23" spans="1:13">
       <c r="A23" s="15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>39</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C23" s="28"/>
       <c r="D23" s="28"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
       <c r="G23" s="28"/>
       <c r="H23" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="I23" s="27"/>
-      <c r="J23" s="15" t="s">
-        <v>20</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="27"/>
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" s="31" customFormat="1">
       <c r="A24" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-    </row>
-    <row r="25" spans="1:13" s="31" customFormat="1">
-      <c r="A25" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="29" t="s">
+      <c r="B24" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="I25" s="29" t="s">
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-    </row>
-    <row r="26" spans="1:13" s="34" customFormat="1">
-      <c r="A26" s="16" t="s">
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+    </row>
+    <row r="25" spans="1:13" s="34" customFormat="1">
+      <c r="A25" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B25" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C25" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
+        <v>124</v>
+      </c>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="15" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
       <c r="G27" s="28"/>
-      <c r="H27" s="16" t="s">
-        <v>131</v>
-      </c>
+      <c r="H27" s="32"/>
       <c r="I27" s="27"/>
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
@@ -1638,14 +1618,10 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>61</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
       <c r="D28" s="28"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
@@ -1659,9 +1635,11 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" s="27"/>
+        <v>62</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>63</v>
+      </c>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
       <c r="E29" s="27"/>
@@ -1676,10 +1654,10 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
@@ -1692,25 +1670,6 @@
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
       <c r="M30" s="27"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1940,10 +1899,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
gw: lf tas update
</commit_message>
<xml_diff>
--- a/LF/TAS/Guinee Bissau/2023/gw_lf_tas1_202310_3_fts_result.xlsx
+++ b/LF/TAS/Guinee Bissau/2023/gw_lf_tas1_202310_3_fts_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Guinee Bissau\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD38544-D7D0-4617-8B5F-A55F9144E05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C0CD9D-55CB-4C55-8032-4DC7C780C976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="127">
   <si>
     <t>type</t>
   </si>
@@ -210,12 +210,6 @@
     <t>O resultado final deste participante é: ${d_final_result}</t>
   </si>
   <si>
-    <t>d_Positivo_why_no_tx</t>
-  </si>
-  <si>
-    <t>Especifique o plano de tratamento deste participante ou explique porque o tratamento não é possível.</t>
-  </si>
-  <si>
     <t>notes_part</t>
   </si>
   <si>
@@ -408,22 +402,19 @@
     <t>selected(${d_why_invalid2},'Other') and ${d_add_results} = 'Sim'</t>
   </si>
   <si>
-    <t>${d_final_result} = 'Positivo' and ${d_add_results} = 'Sim'</t>
-  </si>
-  <si>
     <t>not(selected(${C3}, ${d_code_id}))</t>
   </si>
   <si>
     <t>Este ID já foi introduzido!</t>
   </si>
   <si>
-    <t>(Jan 2024) 3. TAS1 FL - Resultado FTS V1.2</t>
-  </si>
-  <si>
-    <t>gw_lf_tas1_202402_3_fts_result_v1_2</t>
-  </si>
-  <si>
-    <t>gw_fts_202402_v1_2</t>
+    <t>(Jan 2024) 3. TAS1 FL - Resultado FTS V1.3</t>
+  </si>
+  <si>
+    <t>gw_lf_tas1_202402_3_fts_result_v1_3</t>
+  </si>
+  <si>
+    <t>gw_fts_202402_v1_3</t>
   </si>
 </sst>
 </file>
@@ -922,13 +913,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD13"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1027,10 +1018,10 @@
         <v>37</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="15"/>
@@ -1051,7 +1042,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="15"/>
@@ -1074,7 +1065,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="15"/>
@@ -1097,7 +1088,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="15"/>
@@ -1117,7 +1108,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="18"/>
@@ -1126,7 +1117,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="16"/>
       <c r="I7" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -1135,13 +1126,13 @@
     </row>
     <row r="8" spans="1:14" s="12" customFormat="1">
       <c r="A8" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="20"/>
@@ -1160,7 +1151,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
@@ -1169,7 +1160,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="16"/>
       <c r="I9" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
@@ -1181,7 +1172,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
@@ -1190,7 +1181,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="16"/>
       <c r="I10" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
@@ -1199,13 +1190,13 @@
     </row>
     <row r="11" spans="1:14" s="12" customFormat="1">
       <c r="A11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>116</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>118</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="15"/>
@@ -1225,21 +1216,21 @@
         <v>24</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="15" t="s">
@@ -1264,7 +1255,7 @@
       <c r="F13" s="25"/>
       <c r="G13" s="18"/>
       <c r="H13" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="15" t="s">
@@ -1291,7 +1282,7 @@
       <c r="F14" s="15"/>
       <c r="G14" s="26"/>
       <c r="H14" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I14" s="16"/>
       <c r="J14" s="15" t="s">
@@ -1341,7 +1332,7 @@
       <c r="F16" s="15"/>
       <c r="G16" s="26"/>
       <c r="H16" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I16" s="16"/>
       <c r="J16" s="15" t="s">
@@ -1389,7 +1380,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="26"/>
       <c r="H18" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
@@ -1416,7 +1407,7 @@
         <v>28</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15" t="s">
@@ -1443,7 +1434,7 @@
       <c r="F20" s="27"/>
       <c r="G20" s="28"/>
       <c r="H20" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I20" s="27"/>
       <c r="J20" s="15" t="s">
@@ -1468,7 +1459,7 @@
       <c r="F21" s="27"/>
       <c r="G21" s="28"/>
       <c r="H21" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I21" s="27"/>
       <c r="J21" s="15" t="s">
@@ -1493,7 +1484,7 @@
       <c r="F22" s="27"/>
       <c r="G22" s="28"/>
       <c r="H22" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I22" s="27"/>
       <c r="J22" s="15" t="s">
@@ -1516,7 +1507,7 @@
       <c r="F23" s="27"/>
       <c r="G23" s="28"/>
       <c r="H23" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>42</v>
@@ -1539,7 +1530,7 @@
       <c r="F24" s="29"/>
       <c r="G24" s="30"/>
       <c r="H24" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I24" s="29" t="s">
         <v>55</v>
@@ -1564,7 +1555,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
       <c r="H25" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I25" s="32"/>
       <c r="J25" s="32"/>
@@ -1574,7 +1565,7 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="15" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>58</v>
@@ -1586,9 +1577,7 @@
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
       <c r="G26" s="28"/>
-      <c r="H26" s="16" t="s">
-        <v>124</v>
-      </c>
+      <c r="H26" s="32"/>
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
@@ -1597,14 +1586,10 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>61</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="28"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
@@ -1618,9 +1603,11 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28" s="27"/>
+        <v>60</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>61</v>
+      </c>
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
       <c r="E28" s="27"/>
@@ -1651,25 +1638,6 @@
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
       <c r="M29" s="27"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1695,7 +1663,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1706,156 +1674,156 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" t="s">
-        <v>77</v>
-      </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
         <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1885,27 +1853,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>20</v>

</xml_diff>